<commit_message>
Driver timesheet report added
</commit_message>
<xml_diff>
--- a/src/main/resources/driver-timesheet.xlsx
+++ b/src/main/resources/driver-timesheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3EFBBD-11F0-474B-B602-1DADFDC409C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -15,8 +16,19 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Номер маршрута:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата создания отчета: </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,6 +69,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -105,7 +120,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -138,9 +153,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -173,6 +205,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -348,41 +397,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="78" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="9" width="8.83203125" customWidth="1"/>
+    <col min="35" max="36" width="12.83203125" customWidth="1"/>
+    <col min="37" max="37" width="17.83203125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[#5] some updates were made
</commit_message>
<xml_diff>
--- a/src/main/resources/driver-timesheet.xlsx
+++ b/src/main/resources/driver-timesheet.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3EFBBD-11F0-474B-B602-1DADFDC409C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,7 +119,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -153,26 +152,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -205,23 +187,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -397,28 +362,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="9" width="8.83203125" customWidth="1"/>
-    <col min="35" max="36" width="12.83203125" customWidth="1"/>
-    <col min="37" max="37" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="9" width="8.85546875" customWidth="1"/>
+    <col min="35" max="36" width="12.85546875" customWidth="1"/>
+    <col min="37" max="37" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -429,24 +394,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>